<commit_message>
faculty form dbms connected
</commit_message>
<xml_diff>
--- a/Excel and CSV/faculty.xlsx
+++ b/Excel and CSV/faculty.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\WORKSPACE\ARCHIVE PHP MYSQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\arc\Excel and CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418DAEB4-F9C0-4AA5-8103-320D688738EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F55B5D-6D89-4DE8-BFBE-5FC7F9F9E2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5E273C9-C34C-4B19-94CA-0DC1DE5FCAB6}"/>
   </bookViews>
@@ -492,7 +492,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,8 +548,8 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2">
-        <v>36936</v>
+      <c r="D2">
+        <v>2005</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -586,8 +586,8 @@
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2">
-        <v>36926</v>
+      <c r="D3">
+        <v>2006</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -624,8 +624,8 @@
       <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2">
-        <v>36927</v>
+      <c r="D4">
+        <v>2007</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>

</xml_diff>